<commit_message>
Adjust vehicle loading for number of train cars rather than locomotives
</commit_message>
<xml_diff>
--- a/InputData/trans/AVLo/Avg Vehicle Loading.xlsx
+++ b/InputData/trans/AVLo/Avg Vehicle Loading.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\trans\AVLo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-virginia\InputData\trans\AVLo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="114">
   <si>
     <t>AVLo Average Vehicle Loading</t>
   </si>
@@ -372,6 +372,9 @@
   </si>
   <si>
     <t>Vehicle Loading (tons)</t>
+  </si>
+  <si>
+    <t>weighted value, adjusted for number of train cars per locomotive</t>
   </si>
 </sst>
 </file>
@@ -2081,9 +2084,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -2370,224 +2375,233 @@
         <v>48.656731685074099</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="4" t="s">
+    <row r="37" spans="1:3">
+      <c r="A37" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" s="6">
+        <f>B36/10</f>
+        <v>4.8656731685074099</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B39" s="4">
         <v>2005</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>89</v>
-      </c>
-      <c r="B39" s="15">
-        <v>2967</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B40" s="15">
-        <v>100</v>
+        <v>2967</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B41" s="15">
-        <v>27876</v>
-      </c>
-      <c r="C41" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" s="15">
+        <v>27876</v>
+      </c>
+      <c r="C42" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
         <v>96</v>
       </c>
-      <c r="B42" s="15">
+      <c r="B43" s="15">
         <v>4151</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
-      <c r="B43" s="15"/>
-      <c r="C43" t="s">
+    <row r="44" spans="1:3">
+      <c r="B44" s="15"/>
+      <c r="C44" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" s="15">
-        <v>6614973</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B45" s="15">
-        <v>5727512</v>
+        <v>6614973</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B46" s="15">
-        <v>44777151</v>
+        <v>5727512</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="15">
+        <v>44777151</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
         <v>98</v>
       </c>
-      <c r="B47" s="15">
+      <c r="B48" s="15">
         <v>12172542</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
-      <c r="B48" s="15"/>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" t="s">
+    <row r="49" spans="1:2">
+      <c r="B49" s="15"/>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
         <v>93</v>
-      </c>
-      <c r="B49" s="15">
-        <f>B44/B39</f>
-        <v>2229.5156723963601</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" t="s">
-        <v>94</v>
       </c>
       <c r="B50" s="15">
         <f>B45/B40</f>
+        <v>2229.5156723963601</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>94</v>
+      </c>
+      <c r="B51" s="15">
+        <f>B46/B41</f>
         <v>57275.12</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51" t="s">
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
         <v>99</v>
       </c>
-      <c r="B51" s="15">
-        <f t="shared" ref="B51:B52" si="1">B46/B41</f>
+      <c r="B52" s="15">
+        <f t="shared" ref="B52:B53" si="1">B47/B42</f>
         <v>1606.2975678002583</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" t="s">
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
         <v>100</v>
       </c>
-      <c r="B52" s="15">
+      <c r="B53" s="15">
         <f t="shared" si="1"/>
         <v>2932.4360395085523</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="B53" s="15"/>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
+    <row r="54" spans="1:2">
+      <c r="B54" s="15"/>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
         <v>101</v>
       </c>
-      <c r="B54" s="15">
-        <f>SUMPRODUCT(B39:B42,B49:B52)/SUM(B39:B42)</f>
+      <c r="B55" s="15">
+        <f>SUMPRODUCT(B40:B43,B50:B53)/SUM(B40:B43)</f>
         <v>1974.4736422180429</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="B55" s="6"/>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="4" t="s">
+    <row r="56" spans="1:2">
+      <c r="B56" s="6"/>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B56" s="13">
+      <c r="B57" s="13">
         <v>2007</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
         <v>55</v>
       </c>
-      <c r="B57">
+      <c r="B58">
         <v>13611</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="11" t="s">
+    <row r="59" spans="1:2">
+      <c r="A59" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B58" s="11">
+      <c r="B59" s="11">
         <v>17287</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="10" t="s">
+    <row r="60" spans="1:2">
+      <c r="A60" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="7">
-        <f>B58/B57</f>
+      <c r="B60" s="7">
+        <f>B59/B58</f>
         <v>1.2700756740871355</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="10"/>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="4" t="s">
+    <row r="61" spans="1:2">
+      <c r="A61" s="10"/>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B61" s="4">
+      <c r="B62" s="4">
         <v>2007</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
         <v>59</v>
       </c>
-      <c r="B62" s="11">
+      <c r="B63" s="11">
         <v>1670994</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
-      <c r="A63" t="s">
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
         <v>60</v>
       </c>
-      <c r="B63" s="6">
+      <c r="B64" s="6">
         <v>2640170</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" t="s">
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
         <v>61</v>
       </c>
-      <c r="B64" s="7">
-        <f>B63/B62</f>
+      <c r="B65" s="7">
+        <f>B64/B63</f>
         <v>1.579999688807979</v>
       </c>
-      <c r="C64" s="11" t="s">
+      <c r="C65" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="2:2">
-      <c r="B65" s="6"/>
-    </row>
-    <row r="66" spans="2:2">
+    <row r="66" spans="1:3">
       <c r="B66" s="6"/>
     </row>
-    <row r="68" spans="2:2">
-      <c r="B68" s="9"/>
+    <row r="67" spans="1:3">
+      <c r="B67" s="6"/>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="B69" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2605,7 +2619,9 @@
   </sheetPr>
   <dimension ref="A1:AK7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -3177,148 +3193,148 @@
         <v>15</v>
       </c>
       <c r="B5" s="9">
-        <f>'BTS NTS Modal Profile Data'!B36</f>
-        <v>48.656731685074099</v>
+        <f>'BTS NTS Modal Profile Data'!B37</f>
+        <v>4.8656731685074099</v>
       </c>
       <c r="C5" s="7">
         <f t="shared" si="1"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="E5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="G5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="H5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="I5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="J5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="K5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="L5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="M5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="N5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="O5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="P5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="Q5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="R5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="S5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="T5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="U5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="V5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="W5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="X5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="Y5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="Z5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AA5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AB5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AC5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AD5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AE5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AF5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AG5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AH5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AI5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AJ5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AK5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
     </row>
     <row r="6" spans="1:37">
@@ -3474,7 +3490,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="7">
-        <f>'BTS NTS Modal Profile Data'!B59</f>
+        <f>'BTS NTS Modal Profile Data'!B60</f>
         <v>1.2700756740871355</v>
       </c>
       <c r="C7" s="7">
@@ -4330,7 +4346,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="6">
-        <f>'BTS NTS Modal Profile Data'!B54</f>
+        <f>'BTS NTS Modal Profile Data'!B55</f>
         <v>1974.4736422180429</v>
       </c>
       <c r="C6" s="6">

</xml_diff>

<commit_message>
Jun's fixes to rail in transp sector
</commit_message>
<xml_diff>
--- a/InputData/trans/AVLo/Avg Vehicle Loading.xlsx
+++ b/InputData/trans/AVLo/Avg Vehicle Loading.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\trans\AVLo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jshepard/Projects/state-eps-data-repository/VA/trans/AVLo/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF7B83D-0933-0D49-AECC-8D407C64A5D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="19425" windowHeight="11025"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="19420" windowHeight="11020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -28,12 +29,22 @@
     <definedName name="ti_tbl_50">#REF!</definedName>
     <definedName name="ti_tbl_69">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="114">
   <si>
     <t>AVLo Average Vehicle Loading</t>
   </si>
@@ -372,12 +383,15 @@
   </si>
   <si>
     <t>Vehicle Loading (tons)</t>
+  </si>
+  <si>
+    <t>weighted value, adjusted for number of train cars per locomotive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -1280,160 +1294,160 @@
     </xf>
   </cellXfs>
   <cellStyles count="154">
-    <cellStyle name="20% - Accent1 2" xfId="2"/>
-    <cellStyle name="20% - Accent2 2" xfId="3"/>
-    <cellStyle name="20% - Accent3 2" xfId="4"/>
-    <cellStyle name="20% - Accent4 2" xfId="5"/>
-    <cellStyle name="20% - Accent5 2" xfId="6"/>
-    <cellStyle name="20% - Accent6 2" xfId="7"/>
-    <cellStyle name="40% - Accent1 2" xfId="8"/>
-    <cellStyle name="40% - Accent2 2" xfId="9"/>
-    <cellStyle name="40% - Accent3 2" xfId="10"/>
-    <cellStyle name="40% - Accent4 2" xfId="11"/>
-    <cellStyle name="40% - Accent5 2" xfId="12"/>
-    <cellStyle name="40% - Accent6 2" xfId="13"/>
-    <cellStyle name="60% - Accent1 2" xfId="14"/>
-    <cellStyle name="60% - Accent2 2" xfId="15"/>
-    <cellStyle name="60% - Accent3 2" xfId="16"/>
-    <cellStyle name="60% - Accent4 2" xfId="17"/>
-    <cellStyle name="60% - Accent5 2" xfId="18"/>
-    <cellStyle name="60% - Accent6 2" xfId="19"/>
-    <cellStyle name="Accent1 2" xfId="20"/>
-    <cellStyle name="Accent2 2" xfId="21"/>
-    <cellStyle name="Accent3 2" xfId="22"/>
-    <cellStyle name="Accent4 2" xfId="23"/>
-    <cellStyle name="Accent5 2" xfId="24"/>
-    <cellStyle name="Accent6 2" xfId="25"/>
-    <cellStyle name="Bad 2" xfId="26"/>
-    <cellStyle name="Body: normal cell" xfId="27"/>
-    <cellStyle name="Body: normal cell 2" xfId="28"/>
-    <cellStyle name="Calculation 2" xfId="29"/>
-    <cellStyle name="Check Cell 2" xfId="30"/>
-    <cellStyle name="Column heading" xfId="31"/>
-    <cellStyle name="Comma 2" xfId="32"/>
-    <cellStyle name="Comma 2 2" xfId="33"/>
-    <cellStyle name="Comma 3" xfId="34"/>
-    <cellStyle name="Comma 4" xfId="35"/>
-    <cellStyle name="Comma 5" xfId="36"/>
-    <cellStyle name="Comma 6" xfId="37"/>
-    <cellStyle name="Comma 7" xfId="38"/>
-    <cellStyle name="Comma 8" xfId="39"/>
-    <cellStyle name="Corner heading" xfId="40"/>
-    <cellStyle name="Currency 2" xfId="41"/>
-    <cellStyle name="Currency 3" xfId="42"/>
-    <cellStyle name="Currency 3 2" xfId="43"/>
-    <cellStyle name="Data" xfId="44"/>
-    <cellStyle name="Data 2" xfId="45"/>
-    <cellStyle name="Data no deci" xfId="46"/>
-    <cellStyle name="Data Superscript" xfId="47"/>
-    <cellStyle name="Data_1-1A-Regular" xfId="48"/>
-    <cellStyle name="Explanatory Text 2" xfId="49"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="50"/>
-    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="51"/>
-    <cellStyle name="Footnotes: top row" xfId="52"/>
-    <cellStyle name="Footnotes: top row 2" xfId="53"/>
-    <cellStyle name="Good 2" xfId="54"/>
-    <cellStyle name="Header: bottom row" xfId="55"/>
-    <cellStyle name="Header: bottom row 2" xfId="56"/>
-    <cellStyle name="Heading 1 2" xfId="57"/>
-    <cellStyle name="Heading 2 2" xfId="58"/>
-    <cellStyle name="Heading 3 2" xfId="59"/>
-    <cellStyle name="Heading 4 2" xfId="60"/>
-    <cellStyle name="Hed Side" xfId="61"/>
-    <cellStyle name="Hed Side 2" xfId="62"/>
-    <cellStyle name="Hed Side bold" xfId="63"/>
-    <cellStyle name="Hed Side Indent" xfId="64"/>
-    <cellStyle name="Hed Side Regular" xfId="65"/>
-    <cellStyle name="Hed Side_1-1A-Regular" xfId="66"/>
-    <cellStyle name="Hed Top" xfId="67"/>
-    <cellStyle name="Hed Top - SECTION" xfId="68"/>
-    <cellStyle name="Hed Top_3-new4" xfId="69"/>
+    <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="20% - Accent2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - Accent3 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20% - Accent4 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20% - Accent5 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20% - Accent6 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="40% - Accent1 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="40% - Accent2 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="40% - Accent3 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="40% - Accent4 2" xfId="11" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="40% - Accent5 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="40% - Accent6 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="60% - Accent1 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="60% - Accent2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="60% - Accent3 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="60% - Accent4 2" xfId="17" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="60% - Accent5 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="60% - Accent6 2" xfId="19" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Accent1 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Accent2 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Accent3 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Accent4 2" xfId="23" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Accent5 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Accent6 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Bad 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Body: normal cell" xfId="27" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Body: normal cell 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Calculation 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Check Cell 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Column heading" xfId="31" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Comma 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="Comma 2 2" xfId="33" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Comma 3" xfId="34" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Comma 4" xfId="35" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Comma 5" xfId="36" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Comma 6" xfId="37" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Comma 7" xfId="38" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Comma 8" xfId="39" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="Corner heading" xfId="40" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="Currency 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="Currency 3" xfId="42" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="Currency 3 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="Data" xfId="44" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Data 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Data no deci" xfId="46" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="Data Superscript" xfId="47" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="Data_1-1A-Regular" xfId="48" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="Explanatory Text 2" xfId="49" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="50" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="52" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Footnotes: top row 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Good 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Header: bottom row" xfId="55" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Header: bottom row 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Heading 1 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Heading 2 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Heading 3 2" xfId="59" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Heading 4 2" xfId="60" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Hed Side" xfId="61" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Hed Side 2" xfId="62" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Hed Side bold" xfId="63" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Hed Side Indent" xfId="64" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Hed Side Regular" xfId="65" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Hed Side_1-1A-Regular" xfId="66" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="Hed Top" xfId="67" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="Hed Top - SECTION" xfId="68" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="Hed Top_3-new4" xfId="69" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="70"/>
-    <cellStyle name="Input 2" xfId="71"/>
-    <cellStyle name="Linked Cell 2" xfId="72"/>
-    <cellStyle name="Neutral 2" xfId="73"/>
+    <cellStyle name="Hyperlink 2" xfId="70" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="Input 2" xfId="71" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="Linked Cell 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
+    <cellStyle name="Neutral 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="74"/>
-    <cellStyle name="Normal 11" xfId="75"/>
-    <cellStyle name="Normal 2" xfId="76"/>
-    <cellStyle name="Normal 2 2" xfId="77"/>
-    <cellStyle name="Normal 2 3" xfId="78"/>
-    <cellStyle name="Normal 3" xfId="79"/>
-    <cellStyle name="Normal 3 2" xfId="80"/>
-    <cellStyle name="Normal 3 2 2" xfId="81"/>
-    <cellStyle name="Normal 3 2 2 2" xfId="82"/>
-    <cellStyle name="Normal 3 2 3" xfId="83"/>
-    <cellStyle name="Normal 3 3" xfId="84"/>
-    <cellStyle name="Normal 3 3 2" xfId="85"/>
-    <cellStyle name="Normal 3 3 2 2" xfId="86"/>
-    <cellStyle name="Normal 3 3 3" xfId="87"/>
-    <cellStyle name="Normal 3 4" xfId="88"/>
-    <cellStyle name="Normal 3 4 2" xfId="89"/>
-    <cellStyle name="Normal 3 5" xfId="90"/>
-    <cellStyle name="Normal 3 6" xfId="91"/>
-    <cellStyle name="Normal 3 7" xfId="92"/>
-    <cellStyle name="Normal 4" xfId="93"/>
-    <cellStyle name="Normal 4 2" xfId="94"/>
-    <cellStyle name="Normal 4 2 2" xfId="95"/>
-    <cellStyle name="Normal 4 2 2 2" xfId="96"/>
-    <cellStyle name="Normal 4 2 3" xfId="97"/>
-    <cellStyle name="Normal 4 3" xfId="98"/>
-    <cellStyle name="Normal 4 3 2" xfId="99"/>
-    <cellStyle name="Normal 4 3 2 2" xfId="100"/>
-    <cellStyle name="Normal 4 3 3" xfId="101"/>
-    <cellStyle name="Normal 4 4" xfId="102"/>
-    <cellStyle name="Normal 4 4 2" xfId="103"/>
-    <cellStyle name="Normal 4 5" xfId="104"/>
-    <cellStyle name="Normal 4 6" xfId="105"/>
-    <cellStyle name="Normal 4 7" xfId="106"/>
-    <cellStyle name="Normal 5" xfId="107"/>
-    <cellStyle name="Normal 5 2" xfId="108"/>
-    <cellStyle name="Normal 5 3" xfId="109"/>
-    <cellStyle name="Normal 6" xfId="110"/>
-    <cellStyle name="Normal 6 2" xfId="111"/>
-    <cellStyle name="Normal 7" xfId="112"/>
-    <cellStyle name="Normal 7 2" xfId="113"/>
-    <cellStyle name="Normal 8" xfId="114"/>
-    <cellStyle name="Normal 9" xfId="115"/>
-    <cellStyle name="Note 2" xfId="116"/>
-    <cellStyle name="Note 2 2" xfId="117"/>
-    <cellStyle name="Output 2" xfId="118"/>
-    <cellStyle name="Parent row" xfId="119"/>
-    <cellStyle name="Parent row 2" xfId="120"/>
-    <cellStyle name="Percent 2" xfId="121"/>
-    <cellStyle name="Percent 2 2" xfId="122"/>
-    <cellStyle name="Percent 3" xfId="123"/>
-    <cellStyle name="Percent 3 2" xfId="124"/>
-    <cellStyle name="Percent 4" xfId="125"/>
-    <cellStyle name="Reference" xfId="126"/>
-    <cellStyle name="Row heading" xfId="127"/>
-    <cellStyle name="Source Hed" xfId="128"/>
-    <cellStyle name="Source Letter" xfId="129"/>
-    <cellStyle name="Source Superscript" xfId="130"/>
-    <cellStyle name="Source Superscript 2" xfId="131"/>
-    <cellStyle name="Source Text" xfId="132"/>
-    <cellStyle name="Source Text 2" xfId="133"/>
-    <cellStyle name="State" xfId="134"/>
-    <cellStyle name="Superscript" xfId="135"/>
-    <cellStyle name="Table Data" xfId="136"/>
-    <cellStyle name="Table Head Top" xfId="137"/>
-    <cellStyle name="Table Hed Side" xfId="138"/>
-    <cellStyle name="Table title" xfId="139"/>
-    <cellStyle name="Table title 2" xfId="140"/>
-    <cellStyle name="Title 2" xfId="141"/>
-    <cellStyle name="Title Text" xfId="142"/>
-    <cellStyle name="Title Text 1" xfId="143"/>
-    <cellStyle name="Title Text 2" xfId="144"/>
-    <cellStyle name="Title-1" xfId="145"/>
-    <cellStyle name="Title-2" xfId="146"/>
-    <cellStyle name="Title-3" xfId="147"/>
-    <cellStyle name="Total 2" xfId="148"/>
-    <cellStyle name="Warning Text 2" xfId="149"/>
-    <cellStyle name="Wrap" xfId="150"/>
-    <cellStyle name="Wrap Bold" xfId="151"/>
-    <cellStyle name="Wrap Title" xfId="152"/>
-    <cellStyle name="Wrap_NTS99-~11" xfId="153"/>
+    <cellStyle name="Normal 10" xfId="74" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="Normal 11" xfId="75" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
+    <cellStyle name="Normal 2" xfId="76" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
+    <cellStyle name="Normal 2 2" xfId="77" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="Normal 2 3" xfId="78" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
+    <cellStyle name="Normal 3" xfId="79" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
+    <cellStyle name="Normal 3 2" xfId="80" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="Normal 3 2 2" xfId="81" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="Normal 3 2 2 2" xfId="82" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="Normal 3 2 3" xfId="83" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="Normal 3 3" xfId="84" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="Normal 3 3 2" xfId="85" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="Normal 3 3 2 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="Normal 3 3 3" xfId="87" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="Normal 3 4" xfId="88" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="Normal 3 4 2" xfId="89" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="Normal 3 5" xfId="90" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="Normal 3 6" xfId="91" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="Normal 3 7" xfId="92" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
+    <cellStyle name="Normal 4" xfId="93" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
+    <cellStyle name="Normal 4 2" xfId="94" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="Normal 4 2 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="Normal 4 2 2 2" xfId="96" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="Normal 4 2 3" xfId="97" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="Normal 4 3" xfId="98" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="Normal 4 3 2" xfId="99" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="Normal 4 3 2 2" xfId="100" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="Normal 4 3 3" xfId="101" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="Normal 4 4" xfId="102" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
+    <cellStyle name="Normal 4 4 2" xfId="103" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
+    <cellStyle name="Normal 4 5" xfId="104" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="Normal 4 6" xfId="105" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="Normal 4 7" xfId="106" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="Normal 5" xfId="107" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="Normal 5 2" xfId="108" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="Normal 5 3" xfId="109" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="Normal 6" xfId="110" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="Normal 6 2" xfId="111" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="Normal 7" xfId="112" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="Normal 7 2" xfId="113" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="Normal 8" xfId="114" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="Normal 9" xfId="115" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="Note 2" xfId="116" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="Note 2 2" xfId="117" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="Output 2" xfId="118" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="Parent row" xfId="119" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="Parent row 2" xfId="120" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="Percent 2" xfId="121" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
+    <cellStyle name="Percent 2 2" xfId="122" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
+    <cellStyle name="Percent 3" xfId="123" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
+    <cellStyle name="Percent 3 2" xfId="124" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
+    <cellStyle name="Percent 4" xfId="125" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
+    <cellStyle name="Reference" xfId="126" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
+    <cellStyle name="Row heading" xfId="127" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
+    <cellStyle name="Source Hed" xfId="128" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="Source Letter" xfId="129" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="Source Superscript" xfId="130" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="Source Superscript 2" xfId="131" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="Source Text" xfId="132" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="Source Text 2" xfId="133" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
+    <cellStyle name="State" xfId="134" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
+    <cellStyle name="Superscript" xfId="135" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
+    <cellStyle name="Table Data" xfId="136" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
+    <cellStyle name="Table Head Top" xfId="137" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
+    <cellStyle name="Table Hed Side" xfId="138" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
+    <cellStyle name="Table title" xfId="139" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
+    <cellStyle name="Table title 2" xfId="140" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
+    <cellStyle name="Title 2" xfId="141" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
+    <cellStyle name="Title Text" xfId="142" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="Title Text 1" xfId="143" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="Title Text 2" xfId="144" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
+    <cellStyle name="Title-1" xfId="145" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
+    <cellStyle name="Title-2" xfId="146" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
+    <cellStyle name="Title-3" xfId="147" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="Total 2" xfId="148" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
+    <cellStyle name="Warning Text 2" xfId="149" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
+    <cellStyle name="Wrap" xfId="150" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
+    <cellStyle name="Wrap Bold" xfId="151" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
+    <cellStyle name="Wrap Title" xfId="152" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="Wrap_NTS99-~11" xfId="153" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1605,6 +1619,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1640,6 +1671,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1815,17 +1863,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.59765625" customWidth="1"/>
-    <col min="2" max="2" width="85.1328125" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="85.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2071,8 +2119,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B14" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B14" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
@@ -2080,16 +2128,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="73.59765625" customWidth="1"/>
+    <col min="1" max="1" width="73.6640625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="102.265625" customWidth="1"/>
+    <col min="3" max="3" width="102.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2361,7 +2411,7 @@
         <v>33.023738872403563</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" ht="16">
       <c r="A36" s="10" t="s">
         <v>47</v>
       </c>
@@ -2370,224 +2420,233 @@
         <v>48.656731685074099</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="4" t="s">
+    <row r="37" spans="1:3" ht="16">
+      <c r="A37" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B37" s="6">
+        <f>B36/10</f>
+        <v>4.8656731685074099</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B39" s="4">
         <v>2005</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>89</v>
-      </c>
-      <c r="B39" s="15">
-        <v>2967</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B40" s="15">
-        <v>100</v>
+        <v>2967</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B41" s="15">
-        <v>27876</v>
-      </c>
-      <c r="C41" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" s="15">
+        <v>27876</v>
+      </c>
+      <c r="C42" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
         <v>96</v>
       </c>
-      <c r="B42" s="15">
+      <c r="B43" s="15">
         <v>4151</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
-      <c r="B43" s="15"/>
-      <c r="C43" t="s">
+    <row r="44" spans="1:3">
+      <c r="B44" s="15"/>
+      <c r="C44" t="s">
         <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" s="15">
-        <v>6614973</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B45" s="15">
-        <v>5727512</v>
+        <v>6614973</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B46" s="15">
-        <v>44777151</v>
+        <v>5727512</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="15">
+        <v>44777151</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
         <v>98</v>
       </c>
-      <c r="B47" s="15">
+      <c r="B48" s="15">
         <v>12172542</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
-      <c r="B48" s="15"/>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" t="s">
+    <row r="49" spans="1:2">
+      <c r="B49" s="15"/>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
         <v>93</v>
-      </c>
-      <c r="B49" s="15">
-        <f>B44/B39</f>
-        <v>2229.5156723963601</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" t="s">
-        <v>94</v>
       </c>
       <c r="B50" s="15">
         <f>B45/B40</f>
+        <v>2229.5156723963601</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>94</v>
+      </c>
+      <c r="B51" s="15">
+        <f>B46/B41</f>
         <v>57275.12</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51" t="s">
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
         <v>99</v>
       </c>
-      <c r="B51" s="15">
-        <f t="shared" ref="B51:B52" si="1">B46/B41</f>
+      <c r="B52" s="15">
+        <f t="shared" ref="B52:B53" si="1">B47/B42</f>
         <v>1606.2975678002583</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" t="s">
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
         <v>100</v>
       </c>
-      <c r="B52" s="15">
+      <c r="B53" s="15">
         <f t="shared" si="1"/>
         <v>2932.4360395085523</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="B53" s="15"/>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
+    <row r="54" spans="1:2">
+      <c r="B54" s="15"/>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
         <v>101</v>
       </c>
-      <c r="B54" s="15">
-        <f>SUMPRODUCT(B39:B42,B49:B52)/SUM(B39:B42)</f>
+      <c r="B55" s="15">
+        <f>SUMPRODUCT(B40:B43,B50:B53)/SUM(B40:B43)</f>
         <v>1974.4736422180429</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="B55" s="6"/>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="4" t="s">
+    <row r="56" spans="1:2">
+      <c r="B56" s="6"/>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B56" s="13">
+      <c r="B57" s="13">
         <v>2007</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
         <v>55</v>
       </c>
-      <c r="B57">
+      <c r="B58">
         <v>13611</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="11" t="s">
+    <row r="59" spans="1:2">
+      <c r="A59" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B58" s="11">
+      <c r="B59" s="11">
         <v>17287</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="10" t="s">
+    <row r="60" spans="1:2" ht="16">
+      <c r="A60" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="7">
-        <f>B58/B57</f>
+      <c r="B60" s="7">
+        <f>B59/B58</f>
         <v>1.2700756740871355</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="10"/>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="4" t="s">
+    <row r="61" spans="1:2">
+      <c r="A61" s="10"/>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B61" s="4">
+      <c r="B62" s="4">
         <v>2007</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
         <v>59</v>
       </c>
-      <c r="B62" s="11">
+      <c r="B63" s="11">
         <v>1670994</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
-      <c r="A63" t="s">
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
         <v>60</v>
       </c>
-      <c r="B63" s="6">
+      <c r="B64" s="6">
         <v>2640170</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" t="s">
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
         <v>61</v>
       </c>
-      <c r="B64" s="7">
-        <f>B63/B62</f>
+      <c r="B65" s="7">
+        <f>B64/B63</f>
         <v>1.579999688807979</v>
       </c>
-      <c r="C64" s="11" t="s">
+      <c r="C65" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="2:2">
-      <c r="B65" s="6"/>
-    </row>
-    <row r="66" spans="2:2">
+    <row r="66" spans="1:3">
       <c r="B66" s="6"/>
     </row>
-    <row r="68" spans="2:2">
-      <c r="B68" s="9"/>
+    <row r="67" spans="1:3">
+      <c r="B67" s="6"/>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="B69" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2599,21 +2658,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AK7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.1328125" customWidth="1"/>
-    <col min="2" max="2" width="8.73046875" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="42.75">
+    <row r="1" spans="1:37" ht="48">
       <c r="A1" s="19" t="s">
         <v>111</v>
       </c>
@@ -3177,148 +3238,148 @@
         <v>15</v>
       </c>
       <c r="B5" s="9">
-        <f>'BTS NTS Modal Profile Data'!B36</f>
-        <v>48.656731685074099</v>
+        <f>'BTS NTS Modal Profile Data'!B37</f>
+        <v>4.8656731685074099</v>
       </c>
       <c r="C5" s="7">
         <f t="shared" si="1"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="E5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="G5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="H5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="I5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="J5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="K5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="L5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="M5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="N5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="O5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="P5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="Q5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="R5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="S5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="T5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="U5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="V5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="W5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="X5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="Y5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="Z5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AA5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AB5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AC5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AD5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AE5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AF5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AG5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AH5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AI5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AJ5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
       <c r="AK5" s="7">
         <f t="shared" si="0"/>
-        <v>48.656731685074099</v>
+        <v>4.8656731685074099</v>
       </c>
     </row>
     <row r="6" spans="1:37">
@@ -3474,7 +3535,7 @@
         <v>17</v>
       </c>
       <c r="B7" s="7">
-        <f>'BTS NTS Modal Profile Data'!B59</f>
+        <f>'BTS NTS Modal Profile Data'!B60</f>
         <v>1.2700756740871355</v>
       </c>
       <c r="C7" s="7">
@@ -3624,7 +3685,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -3632,12 +3693,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.86328125" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="42.75">
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="32">
       <c r="A1" s="19" t="s">
         <v>112</v>
       </c>
@@ -4330,7 +4391,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="6">
-        <f>'BTS NTS Modal Profile Data'!B54</f>
+        <f>'BTS NTS Modal Profile Data'!B55</f>
         <v>1974.4736422180429</v>
       </c>
       <c r="C6" s="6">

</xml_diff>